<commit_message>
Feat : edit kelas on KRS
</commit_message>
<xml_diff>
--- a/public/template/template_mahasiswa3.xlsx
+++ b/public/template/template_mahasiswa3.xlsx
@@ -1582,12 +1582,12 @@
     <t>HAFIDH</t>
   </si>
   <si>
+    <t>Universitas Pendidikan Indonesia</t>
+  </si>
+  <si>
     <t>MO-002</t>
   </si>
   <si>
-    <t>Universitas Pendidikan Indonesia</t>
-  </si>
-  <si>
     <t>ALI FAHMI</t>
   </si>
   <si>
@@ -1618,10 +1618,10 @@
     <t>AISHA IBU</t>
   </si>
   <si>
+    <t>Universitas Negeri Semarang</t>
+  </si>
+  <si>
     <t>TE-003</t>
-  </si>
-  <si>
-    <t>Universitas Negeri Semarang</t>
   </si>
   <si>
     <t>RINA SETIAWATI</t>
@@ -3129,8 +3129,8 @@
   <sheetPr/>
   <dimension ref="A1:BB11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AE10" sqref="AE10"/>
+    <sheetView tabSelected="1" topLeftCell="AI1" workbookViewId="0">
+      <selection activeCell="AT5" sqref="AT5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
@@ -3791,7 +3791,7 @@
         <v>84</v>
       </c>
       <c r="AT4" s="18" t="s">
-        <v>119</v>
+        <v>85</v>
       </c>
       <c r="AU4" s="21" t="s">
         <v>86</v>
@@ -3803,10 +3803,10 @@
         <v>2002</v>
       </c>
       <c r="AX4" s="21" t="s">
+        <v>119</v>
+      </c>
+      <c r="AY4" s="18" t="s">
         <v>120</v>
-      </c>
-      <c r="AY4" s="18" t="s">
-        <v>119</v>
       </c>
       <c r="AZ4" s="3" t="s">
         <v>107</v>
@@ -3953,7 +3953,7 @@
         <v>84</v>
       </c>
       <c r="AT5" s="18" t="s">
-        <v>131</v>
+        <v>85</v>
       </c>
       <c r="AU5" s="21" t="s">
         <v>86</v>
@@ -3965,10 +3965,10 @@
         <v>2003</v>
       </c>
       <c r="AX5" s="21" t="s">
+        <v>131</v>
+      </c>
+      <c r="AY5" s="18" t="s">
         <v>132</v>
-      </c>
-      <c r="AY5" s="18" t="s">
-        <v>131</v>
       </c>
       <c r="AZ5" s="3" t="s">
         <v>107</v>
@@ -4115,7 +4115,7 @@
         <v>84</v>
       </c>
       <c r="AT6" s="18" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="AU6" s="21" t="s">
         <v>105</v>
@@ -4130,7 +4130,7 @@
         <v>144</v>
       </c>
       <c r="AY6" s="18" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="AZ6" s="3" t="s">
         <v>107</v>
@@ -4439,7 +4439,7 @@
         <v>13</v>
       </c>
       <c r="AT8" s="18" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="AU8" s="21" t="s">
         <v>105</v>
@@ -4454,7 +4454,7 @@
         <v>169</v>
       </c>
       <c r="AY8" s="18" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="AZ8" s="3" t="s">
         <v>107</v>

</xml_diff>